<commit_message>
> Implemented ParallelSelectionSort > Fixed bug with Kernel::setArg(cl_uint, Buffer* buffer)
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Benachrichtigung über Genehmigung des Themas</t>
   </si>
   <si>
-    <t>Anlegen SVN und Verzeichnisstruktur</t>
-  </si>
-  <si>
     <t>Latex einrichten und Bachelorarbeitsvorlage von Burger downloaden</t>
   </si>
   <si>
@@ -34,6 +31,12 @@
   </si>
   <si>
     <t>Aktivität</t>
+  </si>
+  <si>
+    <t>Anlegen SVN und Verzeichnisstruktur, Create project sort, Implement test for own quicksort, c qsort and c++ sort</t>
+  </si>
+  <si>
+    <t>Created OpenCL classes, Implemented Bealto ParallelSelectionSort</t>
   </si>
 </sst>
 </file>
@@ -41,7 +44,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -89,12 +92,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +403,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,10 +414,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -437,7 +441,7 @@
         <v>41112</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -445,7 +449,15 @@
         <v>41113</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>41119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
> Added codeblocks lexer file for OpenCL
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Created OpenCL classes, Implemented Bealto ParallelSelectionSort</t>
+  </si>
+  <si>
+    <t>Implemented Bealto ParallelSelectionSortLocal and ParallelSelectionSortBlocks</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,6 +463,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>41121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>

</xml_diff>

<commit_message>
> Implemented ParallelBitonicSortLocalOptim > Implemented ParallelBitonicSortB2 (running faster than CPU quicksort)
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Implemented Bealto ParallelBitonicSortLocal</t>
+  </si>
+  <si>
+    <t>Implemented Bealto ParallelBitonicSortA, ParallelBitonicSortB2 (first algorithm running faster than CPU Quicksort)</t>
   </si>
 </sst>
 </file>
@@ -408,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,6 +485,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>41123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>

</xml_diff>

<commit_message>
> Implemented ParallelBitonicSortB4 (first running faster than quicksort in release mode)
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -45,7 +45,7 @@
     <t>Implemented Bealto ParallelBitonicSortLocal</t>
   </si>
   <si>
-    <t>Implemented Bealto ParallelBitonicSortA, ParallelBitonicSortB2 (first algorithm running faster than CPU Quicksort)</t>
+    <t>Implemented Bealto ParallelBitonicSortA, ParallelBitonicSortB2 (first algorithm running faster than CPU Quicksort in Debug mode), ParallelBitonicSortB4 (first algorithm running faster than CPU Quicksort in Release mode)</t>
   </si>
 </sst>
 </file>
@@ -412,13 +412,13 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B18" sqref="B17:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="172.85546875" customWidth="1"/>
+    <col min="2" max="2" width="199.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
> Implemented ParallelBitonicSortB8 and ParallelBitonicSortB16 > Added Kernel::getWorkGroupSize()
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Implemented Bealto ParallelBitonicSortA, ParallelBitonicSortB2 (first algorithm running faster than CPU Quicksort in Debug mode), ParallelBitonicSortB4 (first algorithm running faster than CPU Quicksort in Release mode)</t>
+  </si>
+  <si>
+    <t>Implemented ParallelBitonicSortB8, ParallelBitonicSortB16</t>
   </si>
 </sst>
 </file>
@@ -101,13 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -411,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B17:B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +464,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="1">
         <v>41119</v>
       </c>
       <c r="B6" t="s">
@@ -470,7 +472,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="1">
         <v>41121</v>
       </c>
       <c r="B7" t="s">
@@ -478,7 +480,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="1">
         <v>41122</v>
       </c>
       <c r="B8" t="s">
@@ -486,7 +488,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="1">
         <v>41123</v>
       </c>
       <c r="B9" t="s">
@@ -494,7 +496,12 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>41124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
> Implemented LibCL RadixSort, Added some keywords to lexer file, Refactored RUN macros in main
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Implemented Bealto ParallelBitonicSortC, ParallelMergeSort</t>
+  </si>
+  <si>
+    <t>Implemented LibCL RadixSort, Added some keywords to lexer file, Refactored RUN macros in main</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +518,12 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1">
+        <v>41126</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
> Added OpenSSL OpenCL AES Engine implementation from demo found at https://github.com/softboysxp/OpenCL-AES
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Implemented LibCL RadixSort, Added some keywords to lexer file, Refactored RUN macros in main</t>
+  </si>
+  <si>
+    <t>Tried to get OpenSSL custom OpenCL engine running</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +529,12 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>41129</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>

</xml_diff>

<commit_message>
> Implemented AMD BitonicSort
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Tried to get OpenSSL custom OpenCL engine running</t>
+  </si>
+  <si>
+    <t>Implemented AMD BitonicSort</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +540,12 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>41133</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>

</xml_diff>

<commit_message>
> Implemented CPU AES > Added common directory for OpenCL and Timer class
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -60,7 +60,7 @@
     <t>Tried to get OpenSSL custom OpenCL engine running</t>
   </si>
   <si>
-    <t>Implemented AMD BitonicSort and RadixSort</t>
+    <t>Implemented AMD BitonicSort and RadixSort, Got an CPU AES Implementation running</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
> Implemented CPU Scan
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Implemented AMD BitonicSort and RadixSort, Got an CPU AES Implementation running</t>
+  </si>
+  <si>
+    <t>Implemented clpp radix sort (not working), Implemented CPU Scan</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +551,12 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>42228</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>

</xml_diff>

<commit_message>
> Added webarchives folder > Added CommandQueue->flush() > Added roundToMultiple() and changed power2roundUp to use size_t > Major changes to Runner > Made LocalScan recursive
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Added NaiveScan and WorkEfficientScan from Gpu gems 3</t>
+  </si>
+  <si>
+    <t>Added LocalScan from Gpu gems 3</t>
+  </si>
+  <si>
+    <t>Further working on LocalScan</t>
+  </si>
+  <si>
+    <t>LocalScan technically working now, allocation problems with sizes &gt; 2MiB</t>
   </si>
 </sst>
 </file>
@@ -438,7 +447,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,13 +601,28 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1">
+        <v>41162</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1">
+        <v>41163</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1">
+        <v>41164</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>

</xml_diff>

<commit_message>
> Fixed an issue in the OpenCL device information query methods
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>LocalScan technically working now, allocation problems with sizes &gt; 2MiB</t>
+  </si>
+  <si>
+    <t>Fixed an issue in the OpenCL device information query methods</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +628,12 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1">
+        <v>41166</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>

</xml_diff>

<commit_message>
> Broke applying of sums to buffer into several steps to avoid local memory exhaustion. LocalScan works now up to hardware limits.
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -84,7 +84,7 @@
     <t>LocalScan technically working now, allocation problems with sizes &gt; 2MiB</t>
   </si>
   <si>
-    <t>Fixed an issue in the OpenCL device information query methods</t>
+    <t>Fixed an issue in the OpenCL device information query methods, LocalScan works now up to 64M elements (256MiB)</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
> Optimized LocalScan works now.
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Fixed an issue in the OpenCL device information query methods, LocalScan works now up to 64M elements (256MiB)</t>
+  </si>
+  <si>
+    <t>LocalScan with optimized memory access works now. Is somehow still slower =/</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +639,12 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1">
+        <v>41169</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>

</xml_diff>

<commit_message>
> Added webarchives for Bealto OpenCL Sorting
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Ausgabe des Themenkatalogs, Gespräch mit Dobler</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Cleaned up Runner (removed duplicated code), added stats writing to csv, added device info writing to csv</t>
+  </si>
+  <si>
+    <t>Moved Buffer deletions into download method to avoid OUT_OF_RESOURCES</t>
   </si>
 </sst>
 </file>
@@ -164,13 +167,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,12 +719,44 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="1">
         <v>41179</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
       </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>41183</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
began with OpenCL chapter
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Datum</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>wrote subchapter History and Chapter overview, finished first chapter Introduction</t>
+  </si>
+  <si>
+    <t>began with OpenCL chapter</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1079,12 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
+      <c r="A63" s="4">
+        <v>41371</v>
+      </c>
+      <c r="B63" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>

</xml_diff>

<commit_message>
Wrote chapters "What is OpenCL?" and "Components" Added OpenCL UML diagram
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Datum</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>began with OpenCL chapter</t>
+  </si>
+  <si>
+    <t>wrote subchapter What is OpenCL? and Components</t>
   </si>
 </sst>
 </file>
@@ -572,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1090,12 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
+      <c r="A64" s="4">
+        <v>41372</v>
+      </c>
+      <c r="B64" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>

</xml_diff>

<commit_message>
Updated StatsWriter to OpenCL 1.2
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgruber\Desktop\bakk\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Datum</t>
   </si>
@@ -211,6 +216,9 @@
   </si>
   <si>
     <t>wrote subchapter What is OpenCL? and Components</t>
+  </si>
+  <si>
+    <t>Updated device informations queried in StatsWriter to OpenCL 1.2 (not tested)</t>
   </si>
 </sst>
 </file>
@@ -274,7 +282,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -282,14 +290,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -327,9 +338,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,7 +375,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,7 +410,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -576,10 +587,10 @@
   <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625"/>
     <col min="2" max="2" width="200.7109375"/>
@@ -1097,43 +1108,48 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>41373</v>
+      </c>
+      <c r="B65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
     </row>
   </sheetData>
@@ -1148,7 +1164,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1161,7 +1177,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
* Added level 1 & 2 caches to ivy_bridge.png * Finished CPU chapter
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgruber\Desktop\bakk\documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="450" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Datum</t>
   </si>
@@ -219,6 +214,9 @@
   </si>
   <si>
     <t>Updated device informations queried in StatsWriter to OpenCL 1.2 (not tested)</t>
+  </si>
+  <si>
+    <t>Added images of Ivy Bridge and Kepler architecture. Write chapter about CPU.</t>
   </si>
 </sst>
 </file>
@@ -282,7 +280,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -298,9 +296,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -338,9 +336,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,7 +373,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,7 +408,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -587,10 +585,10 @@
   <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625"/>
     <col min="2" max="2" width="200.7109375"/>
@@ -1117,7 +1115,12 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
+      <c r="A66" s="4">
+        <v>41377</v>
+      </c>
+      <c r="B66" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
@@ -1164,7 +1167,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1177,7 +1180,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Finished GPU architecture chapter
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Datum</t>
   </si>
@@ -216,7 +216,10 @@
     <t>Updated device informations queried in StatsWriter to OpenCL 1.2 (not tested)</t>
   </si>
   <si>
-    <t>Added images of Ivy Bridge and Kepler architecture. Write chapter about CPU.</t>
+    <t>Added images of Ivy Bridge and Kepler architecture. Write chapter about CPU hardware architecture</t>
+  </si>
+  <si>
+    <t>Finished chapter about the GPU hardware architecture. Added an additional paper about GPU optimizations</t>
   </si>
 </sst>
 </file>
@@ -585,7 +588,7 @@
   <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1126,12 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
+      <c r="A67" s="4">
+        <v>41378</v>
+      </c>
+      <c r="B67" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>

</xml_diff>

<commit_message>
* Wrote API Overview * Switched to biblatex
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Datum</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Finished chapter about the GPU hardware architecture. Added an additional paper about GPU optimizations</t>
+  </si>
+  <si>
+    <t>Wrote API overview</t>
   </si>
 </sst>
 </file>
@@ -588,7 +591,7 @@
   <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,7 +1137,12 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
+      <c r="A68" s="4">
+        <v>41380</v>
+      </c>
+      <c r="B68" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>

</xml_diff>

<commit_message>
wrote chapter platform model and first part of chapter execution model
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Datum</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>Wrote API overview</t>
+  </si>
+  <si>
+    <t>Wrote chapter platform model and first part of chapter execution model</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
   <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1148,12 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
+      <c r="A69" s="4">
+        <v>41382</v>
+      </c>
+      <c r="B69" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>

</xml_diff>

<commit_message>
* Finished execution model chapter * Wrote memory chapter * Added simple OpenCL demo
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Datum</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>Wrote chapter platform model and first part of chapter execution model</t>
+  </si>
+  <si>
+    <t>Finished execution model chapter, wrote memory chapter, added sample file, FINISHED OPENCL chapter</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
   <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,7 +1159,12 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
+      <c r="A70" s="4">
+        <v>41384</v>
+      </c>
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>

</xml_diff>

<commit_message>
* Proof reading of chapter Introduction and OpenCL * Fixed C::B lexer file * Updated ivy_bridge architecture graphic
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Datum</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Finished execution model chapter, wrote memory chapter, added sample file, FINISHED OPENCL chapter</t>
+  </si>
+  <si>
+    <t>proof-read introduction and OpenCL chapter</t>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
   <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1170,12 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
+      <c r="A71" s="4">
+        <v>41385</v>
+      </c>
+      <c r="B71" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>

</xml_diff>

<commit_message>
wrote naive GPU matrix chapter
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Datum</t>
   </si>
@@ -250,6 +248,9 @@
   </si>
   <si>
     <t>Added new radix sort with devastating performance</t>
+  </si>
+  <si>
+    <t>Wrote naive GPU matrix chapter</t>
   </si>
 </sst>
 </file>
@@ -1244,36 +1245,15 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
+      <c r="A78" s="4">
+        <v>41395</v>
+      </c>
+      <c r="B78" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added benchmark of fastest matrix alg and replaced matrix benchmark chart
</commit_message>
<xml_diff>
--- a/documents/protocol.xlsx
+++ b/documents/protocol.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>Datum</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>Added huge matrix benchmark</t>
+  </si>
+  <si>
+    <t>Added benchmark of fastest matrix alg</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
   <dimension ref="A1:B91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1289,12 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
+      <c r="A82" s="4">
+        <v>41407</v>
+      </c>
+      <c r="B82" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>

</xml_diff>